<commit_message>
Added my info to the RTM report.
</commit_message>
<xml_diff>
--- a/Test Matrix.xlsx
+++ b/Test Matrix.xlsx
@@ -1,11 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24905"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24701"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5571C29B-F28C-4678-9B42-07DAC6FC2F2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kckar\Desktop\Revature\Project-2\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E703C70-AF34-4206-AD21-7F32294FF4E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3390" yWindow="80" windowWidth="15810" windowHeight="7460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="61">
   <si>
     <t>Feature</t>
   </si>
@@ -134,13 +139,88 @@
   </si>
   <si>
     <t>1.1(click on review tab and a list of approved reviews appear if any were approved)</t>
+  </si>
+  <si>
+    <t>Search through books</t>
+  </si>
+  <si>
+    <t>Search through movies</t>
+  </si>
+  <si>
+    <t>Search through games</t>
+  </si>
+  <si>
+    <t>Add new media</t>
+  </si>
+  <si>
+    <t>Approve new media requests</t>
+  </si>
+  <si>
+    <t>Deny new media requests</t>
+  </si>
+  <si>
+    <t>See past media approvals</t>
+  </si>
+  <si>
+    <t>As a user I want to be able to search through books.</t>
+  </si>
+  <si>
+    <t>As a user I want to be able to search through movies.</t>
+  </si>
+  <si>
+    <t>As a user I want to be able to search through games.</t>
+  </si>
+  <si>
+    <t>As a user I want to be able to add new media to my collection.</t>
+  </si>
+  <si>
+    <t>As a moderator I want to approve legitimate media add requests.</t>
+  </si>
+  <si>
+    <t>As a moderator I want to deny legitimate media add requests.</t>
+  </si>
+  <si>
+    <t>As a moderator I want to view my past media approvals.</t>
+  </si>
+  <si>
+    <t>(1.1) Generating list of all books.</t>
+  </si>
+  <si>
+    <t>(1.1) Generating list of all movies.</t>
+  </si>
+  <si>
+    <t>(1.1) Generating list of all games.</t>
+  </si>
+  <si>
+    <t>(1.1) Adding information to add media.</t>
+  </si>
+  <si>
+    <t>(1.1) Entering media id can clicking approve button.</t>
+  </si>
+  <si>
+    <t>(1.1) Entering media id can clicking deny button.</t>
+  </si>
+  <si>
+    <t>(1.1) Generating list of past approved media.</t>
+  </si>
+  <si>
+    <t>(1.2) N/A</t>
+  </si>
+  <si>
+    <t>(1.2) Enter in correct media id.</t>
+  </si>
+  <si>
+    <t>1.1 PASS - 1.2 PASS</t>
+  </si>
+  <si>
+    <t>Kyla Karnoski</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -485,26 +565,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:I15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="I9" sqref="I9:I15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="27.5703125" customWidth="1"/>
-    <col min="2" max="2" width="87.140625" customWidth="1"/>
-    <col min="3" max="3" width="40.28515625" customWidth="1"/>
-    <col min="4" max="4" width="71.42578125" customWidth="1"/>
-    <col min="5" max="5" width="35.7109375" customWidth="1"/>
-    <col min="6" max="6" width="30.28515625" customWidth="1"/>
-    <col min="7" max="7" width="29.42578125" customWidth="1"/>
-    <col min="8" max="8" width="14.7109375" customWidth="1"/>
-    <col min="9" max="9" width="17.140625" customWidth="1"/>
+    <col min="1" max="1" width="27.54296875" customWidth="1"/>
+    <col min="2" max="2" width="87.1796875" customWidth="1"/>
+    <col min="3" max="3" width="40.26953125" customWidth="1"/>
+    <col min="4" max="4" width="71.453125" customWidth="1"/>
+    <col min="5" max="5" width="35.7265625" customWidth="1"/>
+    <col min="6" max="6" width="30.26953125" customWidth="1"/>
+    <col min="7" max="7" width="29.453125" customWidth="1"/>
+    <col min="8" max="8" width="14.7265625" customWidth="1"/>
+    <col min="9" max="9" width="17.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -533,7 +613,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -559,7 +639,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>16</v>
       </c>
@@ -585,7 +665,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>23</v>
       </c>
@@ -611,7 +691,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>26</v>
       </c>
@@ -637,7 +717,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>29</v>
       </c>
@@ -663,7 +743,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>33</v>
       </c>
@@ -687,6 +767,188 @@
       </c>
       <c r="I7" t="s">
         <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>36</v>
+      </c>
+      <c r="B9" t="s">
+        <v>43</v>
+      </c>
+      <c r="D9" t="s">
+        <v>50</v>
+      </c>
+      <c r="E9" t="s">
+        <v>57</v>
+      </c>
+      <c r="F9" t="s">
+        <v>13</v>
+      </c>
+      <c r="G9" t="s">
+        <v>13</v>
+      </c>
+      <c r="H9" t="s">
+        <v>14</v>
+      </c>
+      <c r="I9" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>37</v>
+      </c>
+      <c r="B10" t="s">
+        <v>44</v>
+      </c>
+      <c r="D10" t="s">
+        <v>51</v>
+      </c>
+      <c r="E10" t="s">
+        <v>57</v>
+      </c>
+      <c r="F10" t="s">
+        <v>13</v>
+      </c>
+      <c r="G10" t="s">
+        <v>13</v>
+      </c>
+      <c r="H10" t="s">
+        <v>14</v>
+      </c>
+      <c r="I10" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>38</v>
+      </c>
+      <c r="B11" t="s">
+        <v>45</v>
+      </c>
+      <c r="D11" t="s">
+        <v>52</v>
+      </c>
+      <c r="E11" t="s">
+        <v>57</v>
+      </c>
+      <c r="F11" t="s">
+        <v>13</v>
+      </c>
+      <c r="G11" t="s">
+        <v>13</v>
+      </c>
+      <c r="H11" t="s">
+        <v>14</v>
+      </c>
+      <c r="I11" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>39</v>
+      </c>
+      <c r="B12" t="s">
+        <v>46</v>
+      </c>
+      <c r="D12" t="s">
+        <v>53</v>
+      </c>
+      <c r="E12" t="s">
+        <v>57</v>
+      </c>
+      <c r="F12" t="s">
+        <v>13</v>
+      </c>
+      <c r="G12" t="s">
+        <v>13</v>
+      </c>
+      <c r="H12" t="s">
+        <v>14</v>
+      </c>
+      <c r="I12" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>40</v>
+      </c>
+      <c r="B13" t="s">
+        <v>47</v>
+      </c>
+      <c r="D13" t="s">
+        <v>54</v>
+      </c>
+      <c r="E13" t="s">
+        <v>58</v>
+      </c>
+      <c r="F13" t="s">
+        <v>59</v>
+      </c>
+      <c r="G13" t="s">
+        <v>59</v>
+      </c>
+      <c r="H13" t="s">
+        <v>14</v>
+      </c>
+      <c r="I13" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>41</v>
+      </c>
+      <c r="B14" t="s">
+        <v>48</v>
+      </c>
+      <c r="D14" t="s">
+        <v>55</v>
+      </c>
+      <c r="E14" t="s">
+        <v>57</v>
+      </c>
+      <c r="F14" t="s">
+        <v>13</v>
+      </c>
+      <c r="G14" t="s">
+        <v>13</v>
+      </c>
+      <c r="H14" t="s">
+        <v>14</v>
+      </c>
+      <c r="I14" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>42</v>
+      </c>
+      <c r="B15" t="s">
+        <v>49</v>
+      </c>
+      <c r="D15" t="s">
+        <v>56</v>
+      </c>
+      <c r="E15" t="s">
+        <v>57</v>
+      </c>
+      <c r="F15" t="s">
+        <v>13</v>
+      </c>
+      <c r="G15" t="s">
+        <v>13</v>
+      </c>
+      <c r="H15" t="s">
+        <v>14</v>
+      </c>
+      <c r="I15" t="s">
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>